<commit_message>
añadido .dockerignore y volumen
</commit_message>
<xml_diff>
--- a/config/plantillas_prompts/CU_1_PROMPT_PERTES.xlsx
+++ b/config/plantillas_prompts/CU_1_PROMPT_PERTES.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\server19\Digitalizacion\PROYECTOS INTERNOS\Gestión Documental\FASE II\FASE II - Memorias CDTI\CU1_GENERACION_MEMORIAS\plantillas_prompts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://articaingenieria-my.sharepoint.com/personal/jgarcia_articai_es/Documents/Documentos/GitHub/cu1_gen_memorias/config/plantillas_prompts/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC41A20F-9092-4A9D-A968-B5EB09BDCCCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2EEBB715-0641-4DB6-B9B9-C20CE247016E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2EEBB715-0641-4DB6-B9B9-C20CE247016E}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -667,7 +667,7 @@
   <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>